<commit_message>
Update Master Table data files
- Update Master Table.xlsx with latest data changes
- Add local Master_Table.xlsx copy for ETL processing

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Documents/Prog/Occasional/Parsing Data/Master Table.xlsx
+++ b/Documents/Prog/Occasional/Parsing Data/Master Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haithamdata/Documents/Prog/Occasional/Parsing Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641509EC-F01C-6B49-8CBB-3F9A07D84311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E45082-2A47-434C-9E8C-66D4DBFCE81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="23840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="23840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="45">
   <si>
     <t>Customer</t>
   </si>
@@ -154,12 +154,18 @@
   <si>
     <t>Quarter</t>
   </si>
+  <si>
+    <t>Last month</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +184,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -543,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I193"/>
+  <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -555,13 +567,14 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,20 +590,23 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -603,17 +619,20 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2">
         <v>77143</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>100000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>51473</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -626,14 +645,17 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
         <v>96429</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>125000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -646,14 +668,17 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4">
         <v>96429</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>125000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -666,17 +691,20 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5">
         <v>77143</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>100000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>60253</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -689,17 +717,20 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
         <v>77143</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>100000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>69537</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -712,14 +743,17 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7">
         <v>96429</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>125000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -732,17 +766,20 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8">
         <v>96429</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>125000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>71047</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -755,17 +792,20 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
         <v>77143</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>100000</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>59673</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -778,17 +818,20 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10">
         <v>96429</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>125000</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>75302</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -801,14 +844,17 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11">
         <v>96429</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>125000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -821,14 +867,17 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12">
         <v>96429</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>125000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -841,14 +890,17 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13">
         <v>96429</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>125000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -861,17 +913,20 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14">
         <v>62053</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>80250</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>213253</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -884,14 +939,17 @@
       <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15">
         <v>82737</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>107000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -904,14 +962,17 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16">
         <v>103421</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>133750</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -924,17 +985,20 @@
       <c r="E17" t="s">
         <v>12</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17">
         <v>62053</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>80250</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>85835</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -947,17 +1011,20 @@
       <c r="E18" t="s">
         <v>13</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18">
         <v>62053</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>80250</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>282044</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -970,14 +1037,17 @@
       <c r="E19" t="s">
         <v>14</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19">
         <v>82737</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>107000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -990,17 +1060,20 @@
       <c r="E20" t="s">
         <v>15</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20">
         <v>82737</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>107000</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>124006</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1013,17 +1086,20 @@
       <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21">
         <v>62053</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>80250</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>137944</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1036,17 +1112,20 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22">
         <v>82737</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>107000</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>246026</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1059,14 +1138,17 @@
       <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23">
         <v>103421</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>133750</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1079,14 +1161,17 @@
       <c r="E24" t="s">
         <v>19</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24">
         <v>103421</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>133750</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1099,14 +1184,17 @@
       <c r="E25" t="s">
         <v>20</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25">
         <v>103421</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>133750</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1119,14 +1207,17 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26">
         <v>35145</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>50000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1139,14 +1230,17 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27">
         <v>52717</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>75000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1159,14 +1253,17 @@
       <c r="E28" t="s">
         <v>11</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28">
         <v>52717</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>75000</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1179,14 +1276,17 @@
       <c r="E29" t="s">
         <v>12</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29">
         <v>35145</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>50000</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1199,17 +1299,20 @@
       <c r="E30" t="s">
         <v>13</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30">
         <v>35145</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>50000</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>40464</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1222,14 +1325,17 @@
       <c r="E31" t="s">
         <v>14</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31">
         <v>52717</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>75000</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1242,14 +1348,17 @@
       <c r="E32" t="s">
         <v>15</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32">
         <v>35145</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>50000</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1262,14 +1371,17 @@
       <c r="E33" t="s">
         <v>16</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33">
         <v>35145</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>50000</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1282,14 +1394,17 @@
       <c r="E34" t="s">
         <v>17</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34">
         <v>35145</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>50000</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1302,14 +1417,17 @@
       <c r="E35" t="s">
         <v>18</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35">
         <v>52717</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>75000</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1322,14 +1440,17 @@
       <c r="E36" t="s">
         <v>19</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36">
         <v>52717</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>75000</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1342,14 +1463,17 @@
       <c r="E37" t="s">
         <v>20</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37">
         <v>52717</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>75000</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1362,14 +1486,17 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38">
         <v>41721</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>60000</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1382,14 +1509,17 @@
       <c r="E39" t="s">
         <v>10</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39">
         <v>48675</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>70000</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -1402,14 +1532,17 @@
       <c r="E40" t="s">
         <v>11</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40">
         <v>55629</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>80000</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1422,17 +1555,20 @@
       <c r="E41" t="s">
         <v>12</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41">
         <v>41721</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>60000</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>92651</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -1445,17 +1581,20 @@
       <c r="E42" t="s">
         <v>13</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42">
         <v>41721</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>60000</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>110145</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -1468,14 +1607,17 @@
       <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43">
         <v>48675</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>70000</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -1488,14 +1630,17 @@
       <c r="E44" t="s">
         <v>15</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44">
         <v>48675</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>70000</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -1508,17 +1653,20 @@
       <c r="E45" t="s">
         <v>16</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45">
         <v>41721</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>60000</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>213265</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -1531,14 +1679,17 @@
       <c r="E46" t="s">
         <v>17</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46">
         <v>48675</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>70000</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -1551,14 +1702,17 @@
       <c r="E47" t="s">
         <v>18</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="s">
+        <v>44</v>
+      </c>
+      <c r="G47">
         <v>55629</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>80000</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1571,14 +1725,17 @@
       <c r="E48" t="s">
         <v>19</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48">
         <v>55629</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>80000</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -1591,14 +1748,17 @@
       <c r="E49" t="s">
         <v>20</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49">
         <v>55629</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>80000</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -1611,17 +1771,20 @@
       <c r="E50" t="s">
         <v>9</v>
       </c>
-      <c r="F50">
+      <c r="F50" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50">
         <v>122833</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>152000</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>218768</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1634,14 +1797,17 @@
       <c r="E51" t="s">
         <v>10</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51">
         <v>122833</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>152000</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1654,14 +1820,17 @@
       <c r="E52" t="s">
         <v>11</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52">
         <v>122833</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>152000</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1674,17 +1843,20 @@
       <c r="E53" t="s">
         <v>12</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53">
         <v>122833</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>152000</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>310880</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -1697,17 +1869,20 @@
       <c r="E54" t="s">
         <v>13</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="s">
+        <v>44</v>
+      </c>
+      <c r="G54">
         <v>122833</v>
-      </c>
-      <c r="G54">
-        <v>152000</v>
       </c>
       <c r="H54">
         <v>152000</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <v>152000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -1720,14 +1895,17 @@
       <c r="E55" t="s">
         <v>14</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="s">
+        <v>44</v>
+      </c>
+      <c r="G55">
         <v>122833</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>152000</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -1740,17 +1918,20 @@
       <c r="E56" t="s">
         <v>15</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="s">
+        <v>44</v>
+      </c>
+      <c r="G56">
         <v>122833</v>
-      </c>
-      <c r="G56">
-        <v>152000</v>
       </c>
       <c r="H56">
         <v>152000</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <v>152000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -1763,17 +1944,20 @@
       <c r="E57" t="s">
         <v>16</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="s">
+        <v>44</v>
+      </c>
+      <c r="G57">
         <v>122833</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>152000</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>60000</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -1786,17 +1970,20 @@
       <c r="E58" t="s">
         <v>17</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58">
         <v>122833</v>
-      </c>
-      <c r="G58">
-        <v>152000</v>
       </c>
       <c r="H58">
         <v>152000</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>152000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -1809,14 +1996,17 @@
       <c r="E59" t="s">
         <v>18</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59">
         <v>122833</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>152000</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -1829,14 +2019,17 @@
       <c r="E60" t="s">
         <v>19</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="s">
+        <v>44</v>
+      </c>
+      <c r="G60">
         <v>122833</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>152000</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -1849,14 +2042,17 @@
       <c r="E61" t="s">
         <v>20</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61">
         <v>122833</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>152000</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -1869,17 +2065,20 @@
       <c r="E62" t="s">
         <v>9</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="s">
+        <v>44</v>
+      </c>
+      <c r="G62">
         <v>315124</v>
-      </c>
-      <c r="G62">
-        <v>485000</v>
       </c>
       <c r="H62">
         <v>485000</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>485000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -1892,17 +2091,20 @@
       <c r="E63" t="s">
         <v>10</v>
       </c>
-      <c r="F63">
+      <c r="F63" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63">
         <v>315124</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>485000</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -1915,17 +2117,20 @@
       <c r="E64" t="s">
         <v>11</v>
       </c>
-      <c r="F64">
+      <c r="F64" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64">
         <v>315124</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>485000</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -1938,17 +2143,20 @@
       <c r="E65" t="s">
         <v>12</v>
       </c>
-      <c r="F65">
+      <c r="F65" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65">
         <v>315124</v>
-      </c>
-      <c r="G65">
-        <v>485000</v>
       </c>
       <c r="H65">
         <v>485000</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <v>485000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -1961,17 +2169,20 @@
       <c r="E66" t="s">
         <v>13</v>
       </c>
-      <c r="F66">
+      <c r="F66" t="s">
+        <v>44</v>
+      </c>
+      <c r="G66">
         <v>315124</v>
-      </c>
-      <c r="G66">
-        <v>485000</v>
       </c>
       <c r="H66">
         <v>485000</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66">
+        <v>485000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -1984,17 +2195,20 @@
       <c r="E67" t="s">
         <v>14</v>
       </c>
-      <c r="F67">
+      <c r="F67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67">
         <v>315124</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>485000</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -2007,17 +2221,20 @@
       <c r="E68" t="s">
         <v>15</v>
       </c>
-      <c r="F68">
+      <c r="F68" t="s">
+        <v>44</v>
+      </c>
+      <c r="G68">
         <v>315124</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>485000</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>581200</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -2030,17 +2247,20 @@
       <c r="E69" t="s">
         <v>16</v>
       </c>
-      <c r="F69">
+      <c r="F69" t="s">
+        <v>44</v>
+      </c>
+      <c r="G69">
         <v>315124</v>
-      </c>
-      <c r="G69">
-        <v>485000</v>
       </c>
       <c r="H69">
         <v>485000</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>485000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>24</v>
       </c>
@@ -2053,17 +2273,20 @@
       <c r="E70" t="s">
         <v>17</v>
       </c>
-      <c r="F70">
+      <c r="F70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70">
         <v>315124</v>
-      </c>
-      <c r="G70">
-        <v>485000</v>
       </c>
       <c r="H70">
         <v>485000</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>485000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -2076,17 +2299,20 @@
       <c r="E71" t="s">
         <v>18</v>
       </c>
-      <c r="F71">
+      <c r="F71" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71">
         <v>315124</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>485000</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>24</v>
       </c>
@@ -2099,17 +2325,20 @@
       <c r="E72" t="s">
         <v>19</v>
       </c>
-      <c r="F72">
+      <c r="F72" t="s">
+        <v>44</v>
+      </c>
+      <c r="G72">
         <v>315124</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>485000</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -2122,17 +2351,20 @@
       <c r="E73" t="s">
         <v>20</v>
       </c>
-      <c r="F73">
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73">
         <v>315124</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>485000</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2145,17 +2377,20 @@
       <c r="E74" t="s">
         <v>9</v>
       </c>
-      <c r="F74">
+      <c r="F74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74">
         <v>54479</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>91067</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>35900</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2168,14 +2403,17 @@
       <c r="E75" t="s">
         <v>10</v>
       </c>
-      <c r="F75">
+      <c r="F75" t="s">
+        <v>44</v>
+      </c>
+      <c r="G75">
         <v>105385</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>179317</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -2188,14 +2426,17 @@
       <c r="E76" t="s">
         <v>11</v>
       </c>
-      <c r="F76">
+      <c r="F76" t="s">
+        <v>44</v>
+      </c>
+      <c r="G76">
         <v>128010</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>217567</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -2208,17 +2449,20 @@
       <c r="E77" t="s">
         <v>12</v>
       </c>
-      <c r="F77">
+      <c r="F77" t="s">
+        <v>44</v>
+      </c>
+      <c r="G77">
         <v>54479</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>91067</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>178406</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -2231,17 +2475,20 @@
       <c r="E78" t="s">
         <v>13</v>
       </c>
-      <c r="F78">
+      <c r="F78" t="s">
+        <v>44</v>
+      </c>
+      <c r="G78">
         <v>53546</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>89417</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>141345</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -2254,14 +2501,17 @@
       <c r="E79" t="s">
         <v>14</v>
       </c>
-      <c r="F79">
+      <c r="F79" t="s">
+        <v>44</v>
+      </c>
+      <c r="G79">
         <v>105385</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>179317</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -2274,17 +2524,20 @@
       <c r="E80" t="s">
         <v>15</v>
       </c>
-      <c r="F80">
+      <c r="F80" t="s">
+        <v>44</v>
+      </c>
+      <c r="G80">
         <v>104820</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>178317</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>259668</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -2297,17 +2550,20 @@
       <c r="E81" t="s">
         <v>16</v>
       </c>
-      <c r="F81">
+      <c r="F81" t="s">
+        <v>44</v>
+      </c>
+      <c r="G81">
         <v>54479</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>91067</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>316584</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -2320,17 +2576,20 @@
       <c r="E82" t="s">
         <v>17</v>
       </c>
-      <c r="F82">
+      <c r="F82" t="s">
+        <v>44</v>
+      </c>
+      <c r="G82">
         <v>105385</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>179317</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>262980</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -2343,14 +2602,17 @@
       <c r="E83" t="s">
         <v>18</v>
       </c>
-      <c r="F83">
+      <c r="F83" t="s">
+        <v>44</v>
+      </c>
+      <c r="G83">
         <v>128010</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>217567</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -2363,14 +2625,17 @@
       <c r="E84" t="s">
         <v>19</v>
       </c>
-      <c r="F84">
+      <c r="F84" t="s">
+        <v>44</v>
+      </c>
+      <c r="G84">
         <v>128010</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>217567</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2383,14 +2648,17 @@
       <c r="E85" t="s">
         <v>20</v>
       </c>
-      <c r="F85">
+      <c r="F85" t="s">
+        <v>44</v>
+      </c>
+      <c r="G85">
         <v>128010</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>217567</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -2403,17 +2671,20 @@
       <c r="E86" t="s">
         <v>9</v>
       </c>
-      <c r="F86">
+      <c r="F86" t="s">
+        <v>44</v>
+      </c>
+      <c r="G86">
         <v>563573</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>800000</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>746960</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>27</v>
       </c>
@@ -2426,14 +2697,17 @@
       <c r="E87" t="s">
         <v>10</v>
       </c>
-      <c r="F87">
+      <c r="F87" t="s">
+        <v>44</v>
+      </c>
+      <c r="G87">
         <v>598796</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>850000</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -2446,14 +2720,17 @@
       <c r="E88" t="s">
         <v>11</v>
       </c>
-      <c r="F88">
+      <c r="F88" t="s">
+        <v>44</v>
+      </c>
+      <c r="G88">
         <v>634019</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>900000</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>27</v>
       </c>
@@ -2466,17 +2743,20 @@
       <c r="E89" t="s">
         <v>12</v>
       </c>
-      <c r="F89">
+      <c r="F89" t="s">
+        <v>44</v>
+      </c>
+      <c r="G89">
         <v>563573</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>800000</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>428</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>27</v>
       </c>
@@ -2489,17 +2769,20 @@
       <c r="E90" t="s">
         <v>13</v>
       </c>
-      <c r="F90">
+      <c r="F90" t="s">
+        <v>44</v>
+      </c>
+      <c r="G90">
         <v>563573</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>800000</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>951931</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>27</v>
       </c>
@@ -2512,14 +2795,17 @@
       <c r="E91" t="s">
         <v>14</v>
       </c>
-      <c r="F91">
+      <c r="F91" t="s">
+        <v>44</v>
+      </c>
+      <c r="G91">
         <v>598796</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>850000</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>27</v>
       </c>
@@ -2532,17 +2818,20 @@
       <c r="E92" t="s">
         <v>15</v>
       </c>
-      <c r="F92">
+      <c r="F92" t="s">
+        <v>44</v>
+      </c>
+      <c r="G92">
         <v>598796</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>850000</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <v>771848</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>27</v>
       </c>
@@ -2555,17 +2844,20 @@
       <c r="E93" t="s">
         <v>16</v>
       </c>
-      <c r="F93">
+      <c r="F93" t="s">
+        <v>44</v>
+      </c>
+      <c r="G93">
         <v>563573</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>800000</v>
       </c>
-      <c r="H93">
+      <c r="I93">
         <v>1420844</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>27</v>
       </c>
@@ -2578,17 +2870,20 @@
       <c r="E94" t="s">
         <v>17</v>
       </c>
-      <c r="F94">
+      <c r="F94" t="s">
+        <v>44</v>
+      </c>
+      <c r="G94">
         <v>598796</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>850000</v>
       </c>
-      <c r="H94">
+      <c r="I94">
         <v>623441</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>27</v>
       </c>
@@ -2601,14 +2896,17 @@
       <c r="E95" t="s">
         <v>18</v>
       </c>
-      <c r="F95">
+      <c r="F95" t="s">
+        <v>44</v>
+      </c>
+      <c r="G95">
         <v>634019</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>900000</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>27</v>
       </c>
@@ -2621,14 +2919,17 @@
       <c r="E96" t="s">
         <v>19</v>
       </c>
-      <c r="F96">
+      <c r="F96" t="s">
+        <v>44</v>
+      </c>
+      <c r="G96">
         <v>634019</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>900000</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -2641,14 +2942,17 @@
       <c r="E97" t="s">
         <v>20</v>
       </c>
-      <c r="F97">
+      <c r="F97" t="s">
+        <v>44</v>
+      </c>
+      <c r="G97">
         <v>634019</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>900000</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>27</v>
       </c>
@@ -2661,17 +2965,20 @@
       <c r="E98" t="s">
         <v>9</v>
       </c>
-      <c r="F98">
+      <c r="F98" t="s">
+        <v>44</v>
+      </c>
+      <c r="G98">
         <v>607690</v>
-      </c>
-      <c r="G98">
-        <v>810000</v>
       </c>
       <c r="H98">
         <v>810000</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>27</v>
       </c>
@@ -2684,17 +2991,20 @@
       <c r="E99" t="s">
         <v>10</v>
       </c>
-      <c r="F99">
+      <c r="F99" t="s">
+        <v>44</v>
+      </c>
+      <c r="G99">
         <v>607690</v>
       </c>
-      <c r="G99">
+      <c r="H99">
         <v>810000</v>
       </c>
-      <c r="H99">
+      <c r="I99">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>27</v>
       </c>
@@ -2707,17 +3017,20 @@
       <c r="E100" t="s">
         <v>11</v>
       </c>
-      <c r="F100">
+      <c r="F100" t="s">
+        <v>44</v>
+      </c>
+      <c r="G100">
         <v>607690</v>
       </c>
-      <c r="G100">
+      <c r="H100">
         <v>810000</v>
       </c>
-      <c r="H100">
+      <c r="I100">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -2730,17 +3043,20 @@
       <c r="E101" t="s">
         <v>12</v>
       </c>
-      <c r="F101">
+      <c r="F101" t="s">
+        <v>44</v>
+      </c>
+      <c r="G101">
         <v>607690</v>
-      </c>
-      <c r="G101">
-        <v>810000</v>
       </c>
       <c r="H101">
         <v>810000</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101">
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>27</v>
       </c>
@@ -2753,17 +3069,20 @@
       <c r="E102" t="s">
         <v>13</v>
       </c>
-      <c r="F102">
+      <c r="F102" t="s">
+        <v>44</v>
+      </c>
+      <c r="G102">
         <v>607690</v>
-      </c>
-      <c r="G102">
-        <v>810000</v>
       </c>
       <c r="H102">
         <v>810000</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102">
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>27</v>
       </c>
@@ -2776,17 +3095,20 @@
       <c r="E103" t="s">
         <v>14</v>
       </c>
-      <c r="F103">
+      <c r="F103" t="s">
+        <v>44</v>
+      </c>
+      <c r="G103">
         <v>607690</v>
       </c>
-      <c r="G103">
+      <c r="H103">
         <v>810000</v>
       </c>
-      <c r="H103">
+      <c r="I103">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>27</v>
       </c>
@@ -2799,17 +3121,20 @@
       <c r="E104" t="s">
         <v>15</v>
       </c>
-      <c r="F104">
+      <c r="F104" t="s">
+        <v>44</v>
+      </c>
+      <c r="G104">
         <v>607690</v>
       </c>
-      <c r="G104">
+      <c r="H104">
         <v>810000</v>
       </c>
-      <c r="H104">
+      <c r="I104">
         <v>827078</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>27</v>
       </c>
@@ -2822,17 +3147,20 @@
       <c r="E105" t="s">
         <v>16</v>
       </c>
-      <c r="F105">
+      <c r="F105" t="s">
+        <v>44</v>
+      </c>
+      <c r="G105">
         <v>607690</v>
-      </c>
-      <c r="G105">
-        <v>810000</v>
       </c>
       <c r="H105">
         <v>810000</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105">
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>27</v>
       </c>
@@ -2845,17 +3173,20 @@
       <c r="E106" t="s">
         <v>17</v>
       </c>
-      <c r="F106">
+      <c r="F106" t="s">
+        <v>44</v>
+      </c>
+      <c r="G106">
         <v>607690</v>
-      </c>
-      <c r="G106">
-        <v>810000</v>
       </c>
       <c r="H106">
         <v>810000</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I106">
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -2868,17 +3199,20 @@
       <c r="E107" t="s">
         <v>18</v>
       </c>
-      <c r="F107">
+      <c r="F107" t="s">
+        <v>44</v>
+      </c>
+      <c r="G107">
         <v>607690</v>
       </c>
-      <c r="G107">
+      <c r="H107">
         <v>810000</v>
       </c>
-      <c r="H107">
+      <c r="I107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>27</v>
       </c>
@@ -2891,17 +3225,20 @@
       <c r="E108" t="s">
         <v>19</v>
       </c>
-      <c r="F108">
+      <c r="F108" t="s">
+        <v>44</v>
+      </c>
+      <c r="G108">
         <v>607690</v>
       </c>
-      <c r="G108">
+      <c r="H108">
         <v>810000</v>
       </c>
-      <c r="H108">
+      <c r="I108">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>27</v>
       </c>
@@ -2914,17 +3251,20 @@
       <c r="E109" t="s">
         <v>20</v>
       </c>
-      <c r="F109">
+      <c r="F109" t="s">
+        <v>44</v>
+      </c>
+      <c r="G109">
         <v>607690</v>
       </c>
-      <c r="G109">
+      <c r="H109">
         <v>810000</v>
       </c>
-      <c r="H109">
+      <c r="I109">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>28</v>
       </c>
@@ -2937,17 +3277,20 @@
       <c r="E110" t="s">
         <v>9</v>
       </c>
-      <c r="F110">
+      <c r="F110" t="s">
+        <v>44</v>
+      </c>
+      <c r="G110">
         <v>76763</v>
       </c>
-      <c r="G110">
+      <c r="H110">
         <v>100000</v>
       </c>
-      <c r="H110">
+      <c r="I110">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>28</v>
       </c>
@@ -2960,14 +3303,17 @@
       <c r="E111" t="s">
         <v>10</v>
       </c>
-      <c r="F111">
+      <c r="F111" t="s">
+        <v>44</v>
+      </c>
+      <c r="G111">
         <v>95954</v>
       </c>
-      <c r="G111">
+      <c r="H111">
         <v>125000</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>28</v>
       </c>
@@ -2980,8 +3326,11 @@
       <c r="E112" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>28</v>
       </c>
@@ -2994,17 +3343,20 @@
       <c r="E113" t="s">
         <v>12</v>
       </c>
-      <c r="F113">
+      <c r="F113" t="s">
+        <v>44</v>
+      </c>
+      <c r="G113">
         <v>57572</v>
       </c>
-      <c r="G113">
+      <c r="H113">
         <v>75000</v>
       </c>
-      <c r="H113">
+      <c r="I113">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>28</v>
       </c>
@@ -3017,17 +3369,20 @@
       <c r="E114" t="s">
         <v>13</v>
       </c>
-      <c r="F114">
+      <c r="F114" t="s">
+        <v>44</v>
+      </c>
+      <c r="G114">
         <v>57572</v>
       </c>
-      <c r="G114">
+      <c r="H114">
         <v>75000</v>
       </c>
-      <c r="H114">
+      <c r="I114">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>28</v>
       </c>
@@ -3040,14 +3395,17 @@
       <c r="E115" t="s">
         <v>14</v>
       </c>
-      <c r="F115">
+      <c r="F115" t="s">
+        <v>44</v>
+      </c>
+      <c r="G115">
         <v>95954</v>
       </c>
-      <c r="G115">
+      <c r="H115">
         <v>125000</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>28</v>
       </c>
@@ -3060,14 +3418,17 @@
       <c r="E116" t="s">
         <v>15</v>
       </c>
-      <c r="F116">
+      <c r="F116" t="s">
+        <v>44</v>
+      </c>
+      <c r="G116">
         <v>95954</v>
       </c>
-      <c r="G116">
+      <c r="H116">
         <v>125000</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>28</v>
       </c>
@@ -3080,17 +3441,20 @@
       <c r="E117" t="s">
         <v>16</v>
       </c>
-      <c r="F117">
+      <c r="F117" t="s">
+        <v>44</v>
+      </c>
+      <c r="G117">
         <v>76763</v>
       </c>
-      <c r="G117">
+      <c r="H117">
         <v>100000</v>
       </c>
-      <c r="H117">
+      <c r="I117">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>28</v>
       </c>
@@ -3103,17 +3467,20 @@
       <c r="E118" t="s">
         <v>17</v>
       </c>
-      <c r="F118">
+      <c r="F118" t="s">
+        <v>44</v>
+      </c>
+      <c r="G118">
         <v>76763</v>
       </c>
-      <c r="G118">
+      <c r="H118">
         <v>100000</v>
       </c>
-      <c r="H118">
+      <c r="I118">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>28</v>
       </c>
@@ -3126,8 +3493,11 @@
       <c r="E119" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F119" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>28</v>
       </c>
@@ -3140,8 +3510,11 @@
       <c r="E120" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F120" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3154,14 +3527,17 @@
       <c r="E121" t="s">
         <v>20</v>
       </c>
-      <c r="F121">
+      <c r="F121" t="s">
+        <v>44</v>
+      </c>
+      <c r="G121">
         <v>95954</v>
       </c>
-      <c r="G121">
+      <c r="H121">
         <v>125000</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>29</v>
       </c>
@@ -3174,17 +3550,20 @@
       <c r="E122" t="s">
         <v>9</v>
       </c>
-      <c r="F122">
+      <c r="F122" t="s">
+        <v>44</v>
+      </c>
+      <c r="G122">
         <v>983600</v>
       </c>
-      <c r="G122">
+      <c r="H122">
         <v>1250040</v>
       </c>
-      <c r="H122">
+      <c r="I122">
         <v>1708607</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>29</v>
       </c>
@@ -3197,14 +3576,17 @@
       <c r="E123" t="s">
         <v>10</v>
       </c>
-      <c r="F123">
+      <c r="F123" t="s">
+        <v>44</v>
+      </c>
+      <c r="G123">
         <v>1435478</v>
       </c>
-      <c r="G123">
+      <c r="H123">
         <v>1800150</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -3217,14 +3599,17 @@
       <c r="E124" t="s">
         <v>11</v>
       </c>
-      <c r="F124">
+      <c r="F124" t="s">
+        <v>44</v>
+      </c>
+      <c r="G124">
         <v>1435478</v>
       </c>
-      <c r="G124">
+      <c r="H124">
         <v>1800150</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>29</v>
       </c>
@@ -3237,17 +3622,20 @@
       <c r="E125" t="s">
         <v>12</v>
       </c>
-      <c r="F125">
+      <c r="F125" t="s">
+        <v>44</v>
+      </c>
+      <c r="G125">
         <v>548654</v>
       </c>
-      <c r="G125">
+      <c r="H125">
         <v>675180</v>
       </c>
-      <c r="H125">
+      <c r="I125">
         <v>1154031</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>29</v>
       </c>
@@ -3260,17 +3648,20 @@
       <c r="E126" t="s">
         <v>13</v>
       </c>
-      <c r="F126">
+      <c r="F126" t="s">
+        <v>44</v>
+      </c>
+      <c r="G126">
         <v>242256</v>
       </c>
-      <c r="G126">
+      <c r="H126">
         <v>300630</v>
       </c>
-      <c r="H126">
+      <c r="I126">
         <v>980141</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>29</v>
       </c>
@@ -3283,14 +3674,17 @@
       <c r="E127" t="s">
         <v>14</v>
       </c>
-      <c r="F127">
+      <c r="F127" t="s">
+        <v>44</v>
+      </c>
+      <c r="G127">
         <v>1435478</v>
       </c>
-      <c r="G127">
+      <c r="H127">
         <v>1800150</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>29</v>
       </c>
@@ -3303,14 +3697,17 @@
       <c r="E128" t="s">
         <v>15</v>
       </c>
-      <c r="F128">
+      <c r="F128" t="s">
+        <v>44</v>
+      </c>
+      <c r="G128">
         <v>1229131</v>
       </c>
-      <c r="G128">
+      <c r="H128">
         <v>1549350</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>29</v>
       </c>
@@ -3323,17 +3720,20 @@
       <c r="E129" t="s">
         <v>16</v>
       </c>
-      <c r="F129">
+      <c r="F129" t="s">
+        <v>44</v>
+      </c>
+      <c r="G129">
         <v>797937</v>
       </c>
-      <c r="G129">
+      <c r="H129">
         <v>1001880</v>
       </c>
-      <c r="H129">
+      <c r="I129">
         <v>1397330</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>29</v>
       </c>
@@ -3346,14 +3746,17 @@
       <c r="E130" t="s">
         <v>17</v>
       </c>
-      <c r="F130">
+      <c r="F130" t="s">
+        <v>44</v>
+      </c>
+      <c r="G130">
         <v>1046977</v>
       </c>
-      <c r="G130">
+      <c r="H130">
         <v>1337160</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>29</v>
       </c>
@@ -3366,14 +3769,17 @@
       <c r="E131" t="s">
         <v>18</v>
       </c>
-      <c r="F131">
+      <c r="F131" t="s">
+        <v>44</v>
+      </c>
+      <c r="G131">
         <v>1435478</v>
       </c>
-      <c r="G131">
+      <c r="H131">
         <v>1800150</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>29</v>
       </c>
@@ -3386,14 +3792,17 @@
       <c r="E132" t="s">
         <v>19</v>
       </c>
-      <c r="F132">
+      <c r="F132" t="s">
+        <v>44</v>
+      </c>
+      <c r="G132">
         <v>1435478</v>
       </c>
-      <c r="G132">
+      <c r="H132">
         <v>1800150</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>29</v>
       </c>
@@ -3406,14 +3815,17 @@
       <c r="E133" t="s">
         <v>20</v>
       </c>
-      <c r="F133">
+      <c r="F133" t="s">
+        <v>44</v>
+      </c>
+      <c r="G133">
         <v>1435478</v>
       </c>
-      <c r="G133">
+      <c r="H133">
         <v>1800150</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -3426,17 +3838,20 @@
       <c r="E134" t="s">
         <v>9</v>
       </c>
-      <c r="F134">
+      <c r="F134" t="s">
+        <v>44</v>
+      </c>
+      <c r="G134">
         <v>225000</v>
       </c>
-      <c r="G134">
+      <c r="H134">
         <v>300000</v>
       </c>
-      <c r="H134">
+      <c r="I134">
         <v>339007</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>30</v>
       </c>
@@ -3449,14 +3864,17 @@
       <c r="E135" t="s">
         <v>10</v>
       </c>
-      <c r="F135">
+      <c r="F135" t="s">
+        <v>44</v>
+      </c>
+      <c r="G135">
         <v>300000</v>
       </c>
-      <c r="G135">
+      <c r="H135">
         <v>400000</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -3469,14 +3887,17 @@
       <c r="E136" t="s">
         <v>11</v>
       </c>
-      <c r="F136">
+      <c r="F136" t="s">
+        <v>44</v>
+      </c>
+      <c r="G136">
         <v>375000</v>
       </c>
-      <c r="G136">
+      <c r="H136">
         <v>500000</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>30</v>
       </c>
@@ -3489,17 +3910,20 @@
       <c r="E137" t="s">
         <v>12</v>
       </c>
-      <c r="F137">
+      <c r="F137" t="s">
+        <v>44</v>
+      </c>
+      <c r="G137">
         <v>225000</v>
       </c>
-      <c r="G137">
+      <c r="H137">
         <v>300000</v>
       </c>
-      <c r="H137">
+      <c r="I137">
         <v>241619</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -3512,17 +3936,20 @@
       <c r="E138" t="s">
         <v>13</v>
       </c>
-      <c r="F138">
+      <c r="F138" t="s">
+        <v>44</v>
+      </c>
+      <c r="G138">
         <v>225000</v>
       </c>
-      <c r="G138">
+      <c r="H138">
         <v>300000</v>
       </c>
-      <c r="H138">
+      <c r="I138">
         <v>258565</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>30</v>
       </c>
@@ -3535,14 +3962,17 @@
       <c r="E139" t="s">
         <v>14</v>
       </c>
-      <c r="F139">
+      <c r="F139" t="s">
+        <v>44</v>
+      </c>
+      <c r="G139">
         <v>300000</v>
       </c>
-      <c r="G139">
+      <c r="H139">
         <v>400000</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>30</v>
       </c>
@@ -3555,17 +3985,20 @@
       <c r="E140" t="s">
         <v>15</v>
       </c>
-      <c r="F140">
+      <c r="F140" t="s">
+        <v>44</v>
+      </c>
+      <c r="G140">
         <v>300000</v>
       </c>
-      <c r="G140">
+      <c r="H140">
         <v>400000</v>
       </c>
-      <c r="H140">
+      <c r="I140">
         <v>322340</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -3578,17 +4011,20 @@
       <c r="E141" t="s">
         <v>16</v>
       </c>
-      <c r="F141">
+      <c r="F141" t="s">
+        <v>44</v>
+      </c>
+      <c r="G141">
         <v>225000</v>
       </c>
-      <c r="G141">
+      <c r="H141">
         <v>300000</v>
       </c>
-      <c r="H141">
+      <c r="I141">
         <v>463948</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>30</v>
       </c>
@@ -3601,17 +4037,20 @@
       <c r="E142" t="s">
         <v>17</v>
       </c>
-      <c r="F142">
+      <c r="F142" t="s">
+        <v>44</v>
+      </c>
+      <c r="G142">
         <v>300000</v>
       </c>
-      <c r="G142">
+      <c r="H142">
         <v>400000</v>
       </c>
-      <c r="H142">
+      <c r="I142">
         <v>236014</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>30</v>
       </c>
@@ -3624,14 +4063,17 @@
       <c r="E143" t="s">
         <v>18</v>
       </c>
-      <c r="F143">
+      <c r="F143" t="s">
+        <v>44</v>
+      </c>
+      <c r="G143">
         <v>375000</v>
       </c>
-      <c r="G143">
+      <c r="H143">
         <v>500000</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -3644,14 +4086,17 @@
       <c r="E144" t="s">
         <v>19</v>
       </c>
-      <c r="F144">
+      <c r="F144" t="s">
+        <v>44</v>
+      </c>
+      <c r="G144">
         <v>375000</v>
       </c>
-      <c r="G144">
+      <c r="H144">
         <v>500000</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>30</v>
       </c>
@@ -3664,14 +4109,17 @@
       <c r="E145" t="s">
         <v>20</v>
       </c>
-      <c r="F145">
+      <c r="F145" t="s">
+        <v>44</v>
+      </c>
+      <c r="G145">
         <v>375000</v>
       </c>
-      <c r="G145">
+      <c r="H145">
         <v>500000</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -3684,17 +4132,20 @@
       <c r="E146" t="s">
         <v>9</v>
       </c>
-      <c r="F146">
+      <c r="F146" t="s">
+        <v>44</v>
+      </c>
+      <c r="G146">
         <v>85371</v>
       </c>
-      <c r="G146">
+      <c r="H146">
         <v>114000</v>
       </c>
-      <c r="H146">
+      <c r="I146">
         <v>114650</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>31</v>
       </c>
@@ -3707,14 +4158,17 @@
       <c r="E147" t="s">
         <v>10</v>
       </c>
-      <c r="F147">
+      <c r="F147" t="s">
+        <v>44</v>
+      </c>
+      <c r="G147">
         <v>85371</v>
       </c>
-      <c r="G147">
+      <c r="H147">
         <v>114000</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -3727,8 +4181,11 @@
       <c r="E148" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F148" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>31</v>
       </c>
@@ -3741,17 +4198,20 @@
       <c r="E149" t="s">
         <v>12</v>
       </c>
-      <c r="F149">
+      <c r="F149" t="s">
+        <v>44</v>
+      </c>
+      <c r="G149">
         <v>85371</v>
       </c>
-      <c r="G149">
+      <c r="H149">
         <v>114000</v>
       </c>
-      <c r="H149">
+      <c r="I149">
         <v>229300</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>31</v>
       </c>
@@ -3764,17 +4224,20 @@
       <c r="E150" t="s">
         <v>13</v>
       </c>
-      <c r="F150">
+      <c r="F150" t="s">
+        <v>44</v>
+      </c>
+      <c r="G150">
         <v>85371</v>
       </c>
-      <c r="G150">
+      <c r="H150">
         <v>114000</v>
       </c>
-      <c r="H150">
+      <c r="I150">
         <v>57325</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>31</v>
       </c>
@@ -3787,14 +4250,17 @@
       <c r="E151" t="s">
         <v>14</v>
       </c>
-      <c r="F151">
+      <c r="F151" t="s">
+        <v>44</v>
+      </c>
+      <c r="G151">
         <v>85371</v>
       </c>
-      <c r="G151">
+      <c r="H151">
         <v>114000</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>31</v>
       </c>
@@ -3807,14 +4273,17 @@
       <c r="E152" t="s">
         <v>15</v>
       </c>
-      <c r="F152">
+      <c r="F152" t="s">
+        <v>44</v>
+      </c>
+      <c r="G152">
         <v>85371</v>
       </c>
-      <c r="G152">
+      <c r="H152">
         <v>114000</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>31</v>
       </c>
@@ -3827,17 +4296,20 @@
       <c r="E153" t="s">
         <v>16</v>
       </c>
-      <c r="F153">
+      <c r="F153" t="s">
+        <v>44</v>
+      </c>
+      <c r="G153">
         <v>85371</v>
       </c>
-      <c r="G153">
+      <c r="H153">
         <v>114000</v>
       </c>
-      <c r="H153">
+      <c r="I153">
         <v>114650</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>31</v>
       </c>
@@ -3850,14 +4322,17 @@
       <c r="E154" t="s">
         <v>17</v>
       </c>
-      <c r="F154">
+      <c r="F154" t="s">
+        <v>44</v>
+      </c>
+      <c r="G154">
         <v>85371</v>
       </c>
-      <c r="G154">
+      <c r="H154">
         <v>114000</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>31</v>
       </c>
@@ -3870,14 +4345,17 @@
       <c r="E155" t="s">
         <v>18</v>
       </c>
-      <c r="F155">
+      <c r="F155" t="s">
+        <v>44</v>
+      </c>
+      <c r="G155">
         <v>85371</v>
       </c>
-      <c r="G155">
+      <c r="H155">
         <v>114000</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>31</v>
       </c>
@@ -3890,14 +4368,17 @@
       <c r="E156" t="s">
         <v>19</v>
       </c>
-      <c r="F156">
+      <c r="F156" t="s">
+        <v>44</v>
+      </c>
+      <c r="G156">
         <v>85371</v>
       </c>
-      <c r="G156">
+      <c r="H156">
         <v>114000</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>31</v>
       </c>
@@ -3910,14 +4391,17 @@
       <c r="E157" t="s">
         <v>20</v>
       </c>
-      <c r="F157">
+      <c r="F157" t="s">
+        <v>44</v>
+      </c>
+      <c r="G157">
         <v>85371</v>
       </c>
-      <c r="G157">
+      <c r="H157">
         <v>114000</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>31</v>
       </c>
@@ -3930,17 +4414,20 @@
       <c r="E158" t="s">
         <v>9</v>
       </c>
-      <c r="F158">
+      <c r="F158" t="s">
+        <v>44</v>
+      </c>
+      <c r="G158">
         <v>148940</v>
       </c>
-      <c r="G158">
+      <c r="H158">
         <v>210350</v>
       </c>
-      <c r="H158">
+      <c r="I158">
         <v>420700</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>31</v>
       </c>
@@ -3953,17 +4440,20 @@
       <c r="E159" t="s">
         <v>10</v>
       </c>
-      <c r="F159">
+      <c r="F159" t="s">
+        <v>44</v>
+      </c>
+      <c r="G159">
         <v>148940</v>
       </c>
-      <c r="G159">
+      <c r="H159">
         <v>210350</v>
       </c>
-      <c r="H159">
+      <c r="I159">
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>31</v>
       </c>
@@ -3976,14 +4466,17 @@
       <c r="E160" t="s">
         <v>11</v>
       </c>
-      <c r="G160">
+      <c r="F160" t="s">
+        <v>44</v>
+      </c>
+      <c r="H160">
         <v>210350</v>
       </c>
-      <c r="H160">
+      <c r="I160">
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>31</v>
       </c>
@@ -3996,17 +4489,20 @@
       <c r="E161" t="s">
         <v>12</v>
       </c>
-      <c r="F161">
+      <c r="F161" t="s">
+        <v>44</v>
+      </c>
+      <c r="G161">
         <v>148940</v>
       </c>
-      <c r="G161">
+      <c r="H161">
         <v>210350</v>
       </c>
-      <c r="H161">
+      <c r="I161">
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>31</v>
       </c>
@@ -4019,17 +4515,20 @@
       <c r="E162" t="s">
         <v>13</v>
       </c>
-      <c r="F162">
+      <c r="F162" t="s">
+        <v>44</v>
+      </c>
+      <c r="G162">
         <v>148940</v>
-      </c>
-      <c r="G162">
-        <v>0</v>
       </c>
       <c r="H162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>31</v>
       </c>
@@ -4042,17 +4541,20 @@
       <c r="E163" t="s">
         <v>14</v>
       </c>
-      <c r="F163">
+      <c r="F163" t="s">
+        <v>44</v>
+      </c>
+      <c r="G163">
         <v>148940</v>
       </c>
-      <c r="G163">
+      <c r="H163">
         <v>210350</v>
       </c>
-      <c r="H163">
+      <c r="I163">
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>31</v>
       </c>
@@ -4065,17 +4567,20 @@
       <c r="E164" t="s">
         <v>15</v>
       </c>
-      <c r="F164">
+      <c r="F164" t="s">
+        <v>44</v>
+      </c>
+      <c r="G164">
         <v>148940</v>
-      </c>
-      <c r="G164">
-        <v>210350</v>
       </c>
       <c r="H164">
         <v>210350</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I164">
+        <v>210350</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>31</v>
       </c>
@@ -4088,17 +4593,20 @@
       <c r="E165" t="s">
         <v>16</v>
       </c>
-      <c r="F165">
+      <c r="F165" t="s">
+        <v>44</v>
+      </c>
+      <c r="G165">
         <v>148940</v>
       </c>
-      <c r="G165">
+      <c r="H165">
         <v>210350</v>
       </c>
-      <c r="H165">
+      <c r="I165">
         <v>142675</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>31</v>
       </c>
@@ -4111,17 +4619,20 @@
       <c r="E166" t="s">
         <v>17</v>
       </c>
-      <c r="F166">
+      <c r="F166" t="s">
+        <v>44</v>
+      </c>
+      <c r="G166">
         <v>148940</v>
-      </c>
-      <c r="G166">
-        <v>210350</v>
       </c>
       <c r="H166">
         <v>210350</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I166">
+        <v>210350</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>31</v>
       </c>
@@ -4134,17 +4645,20 @@
       <c r="E167" t="s">
         <v>18</v>
       </c>
-      <c r="F167">
+      <c r="F167" t="s">
+        <v>44</v>
+      </c>
+      <c r="G167">
         <v>148940</v>
       </c>
-      <c r="G167">
+      <c r="H167">
         <v>210350</v>
       </c>
-      <c r="H167">
+      <c r="I167">
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>31</v>
       </c>
@@ -4157,17 +4671,20 @@
       <c r="E168" t="s">
         <v>19</v>
       </c>
-      <c r="F168">
+      <c r="F168" t="s">
+        <v>44</v>
+      </c>
+      <c r="G168">
         <v>148940</v>
       </c>
-      <c r="G168">
+      <c r="H168">
         <v>210350</v>
       </c>
-      <c r="H168">
+      <c r="I168">
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>31</v>
       </c>
@@ -4180,17 +4697,20 @@
       <c r="E169" t="s">
         <v>20</v>
       </c>
-      <c r="F169">
+      <c r="F169" t="s">
+        <v>44</v>
+      </c>
+      <c r="G169">
         <v>148940</v>
       </c>
-      <c r="G169">
+      <c r="H169">
         <v>210350</v>
       </c>
-      <c r="H169">
+      <c r="I169">
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>32</v>
       </c>
@@ -4203,14 +4723,17 @@
       <c r="E170" t="s">
         <v>9</v>
       </c>
-      <c r="F170">
+      <c r="F170" t="s">
+        <v>44</v>
+      </c>
+      <c r="G170">
         <v>40756</v>
       </c>
-      <c r="G170">
+      <c r="H170">
         <v>60000</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>32</v>
       </c>
@@ -4223,14 +4746,17 @@
       <c r="E171" t="s">
         <v>10</v>
       </c>
-      <c r="F171">
+      <c r="F171" t="s">
+        <v>44</v>
+      </c>
+      <c r="G171">
         <v>47548</v>
       </c>
-      <c r="G171">
+      <c r="H171">
         <v>70000</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>32</v>
       </c>
@@ -4243,14 +4769,17 @@
       <c r="E172" t="s">
         <v>11</v>
       </c>
-      <c r="F172">
+      <c r="F172" t="s">
+        <v>44</v>
+      </c>
+      <c r="G172">
         <v>54341</v>
       </c>
-      <c r="G172">
+      <c r="H172">
         <v>80000</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>32</v>
       </c>
@@ -4263,17 +4792,20 @@
       <c r="E173" t="s">
         <v>12</v>
       </c>
-      <c r="F173">
+      <c r="F173" t="s">
+        <v>44</v>
+      </c>
+      <c r="G173">
         <v>40756</v>
       </c>
-      <c r="G173">
+      <c r="H173">
         <v>60000</v>
       </c>
-      <c r="H173">
+      <c r="I173">
         <v>20325</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>32</v>
       </c>
@@ -4286,17 +4818,20 @@
       <c r="E174" t="s">
         <v>13</v>
       </c>
-      <c r="F174">
+      <c r="F174" t="s">
+        <v>44</v>
+      </c>
+      <c r="G174">
         <v>40756</v>
       </c>
-      <c r="G174">
+      <c r="H174">
         <v>60000</v>
       </c>
-      <c r="H174">
+      <c r="I174">
         <v>44617</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>32</v>
       </c>
@@ -4309,14 +4844,17 @@
       <c r="E175" t="s">
         <v>14</v>
       </c>
-      <c r="F175">
+      <c r="F175" t="s">
+        <v>44</v>
+      </c>
+      <c r="G175">
         <v>47548</v>
       </c>
-      <c r="G175">
+      <c r="H175">
         <v>70000</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>32</v>
       </c>
@@ -4329,14 +4867,17 @@
       <c r="E176" t="s">
         <v>15</v>
       </c>
-      <c r="F176">
+      <c r="F176" t="s">
+        <v>44</v>
+      </c>
+      <c r="G176">
         <v>47548</v>
       </c>
-      <c r="G176">
+      <c r="H176">
         <v>70000</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>32</v>
       </c>
@@ -4349,17 +4890,20 @@
       <c r="E177" t="s">
         <v>16</v>
       </c>
-      <c r="F177">
+      <c r="F177" t="s">
+        <v>44</v>
+      </c>
+      <c r="G177">
         <v>40756</v>
       </c>
-      <c r="G177">
+      <c r="H177">
         <v>60000</v>
       </c>
-      <c r="H177">
+      <c r="I177">
         <v>-850</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>32</v>
       </c>
@@ -4372,14 +4916,17 @@
       <c r="E178" t="s">
         <v>17</v>
       </c>
-      <c r="F178">
+      <c r="F178" t="s">
+        <v>44</v>
+      </c>
+      <c r="G178">
         <v>47548</v>
       </c>
-      <c r="G178">
+      <c r="H178">
         <v>70000</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>32</v>
       </c>
@@ -4392,14 +4939,17 @@
       <c r="E179" t="s">
         <v>18</v>
       </c>
-      <c r="F179">
+      <c r="F179" t="s">
+        <v>44</v>
+      </c>
+      <c r="G179">
         <v>54341</v>
       </c>
-      <c r="G179">
+      <c r="H179">
         <v>80000</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>32</v>
       </c>
@@ -4412,14 +4962,17 @@
       <c r="E180" t="s">
         <v>19</v>
       </c>
-      <c r="F180">
+      <c r="F180" t="s">
+        <v>44</v>
+      </c>
+      <c r="G180">
         <v>54341</v>
       </c>
-      <c r="G180">
+      <c r="H180">
         <v>80000</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>32</v>
       </c>
@@ -4432,14 +4985,17 @@
       <c r="E181" t="s">
         <v>20</v>
       </c>
-      <c r="F181">
+      <c r="F181" t="s">
+        <v>44</v>
+      </c>
+      <c r="G181">
         <v>54341</v>
       </c>
-      <c r="G181">
+      <c r="H181">
         <v>80000</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>33</v>
       </c>
@@ -4452,17 +5008,20 @@
       <c r="E182" t="s">
         <v>9</v>
       </c>
-      <c r="F182">
+      <c r="F182" t="s">
+        <v>44</v>
+      </c>
+      <c r="G182">
         <v>165583</v>
       </c>
-      <c r="G182">
+      <c r="H182">
         <v>449808</v>
       </c>
-      <c r="H182">
+      <c r="I182">
         <v>183368</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -4475,17 +5034,20 @@
       <c r="E183" t="s">
         <v>10</v>
       </c>
-      <c r="F183">
+      <c r="F183" t="s">
+        <v>44</v>
+      </c>
+      <c r="G183">
         <v>165583</v>
       </c>
-      <c r="G183">
+      <c r="H183">
         <v>349808</v>
       </c>
-      <c r="H183">
+      <c r="I183">
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>33</v>
       </c>
@@ -4498,17 +5060,20 @@
       <c r="E184" t="s">
         <v>11</v>
       </c>
-      <c r="F184">
+      <c r="F184" t="s">
+        <v>44</v>
+      </c>
+      <c r="G184">
         <v>165583</v>
       </c>
-      <c r="G184">
+      <c r="H184">
         <v>399808</v>
       </c>
-      <c r="H184">
+      <c r="I184">
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>33</v>
       </c>
@@ -4521,17 +5086,20 @@
       <c r="E185" t="s">
         <v>12</v>
       </c>
-      <c r="F185">
+      <c r="F185" t="s">
+        <v>44</v>
+      </c>
+      <c r="G185">
         <v>165583</v>
       </c>
-      <c r="G185">
+      <c r="H185">
         <v>490000</v>
       </c>
-      <c r="H185">
+      <c r="I185">
         <v>339855</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>33</v>
       </c>
@@ -4544,17 +5112,20 @@
       <c r="E186" t="s">
         <v>13</v>
       </c>
-      <c r="F186">
+      <c r="F186" t="s">
+        <v>44</v>
+      </c>
+      <c r="G186">
         <v>165583</v>
       </c>
-      <c r="G186">
+      <c r="H186">
         <v>540000</v>
       </c>
-      <c r="H186">
+      <c r="I186">
         <v>322662</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>33</v>
       </c>
@@ -4567,17 +5138,20 @@
       <c r="E187" t="s">
         <v>14</v>
       </c>
-      <c r="F187">
+      <c r="F187" t="s">
+        <v>44</v>
+      </c>
+      <c r="G187">
         <v>165583</v>
       </c>
-      <c r="G187">
+      <c r="H187">
         <v>449808</v>
       </c>
-      <c r="H187">
+      <c r="I187">
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>33</v>
       </c>
@@ -4590,17 +5164,20 @@
       <c r="E188" t="s">
         <v>15</v>
       </c>
-      <c r="F188">
+      <c r="F188" t="s">
+        <v>44</v>
+      </c>
+      <c r="G188">
         <v>165583</v>
       </c>
-      <c r="G188">
+      <c r="H188">
         <v>399808</v>
       </c>
-      <c r="H188">
+      <c r="I188">
         <v>191906</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>33</v>
       </c>
@@ -4613,17 +5190,20 @@
       <c r="E189" t="s">
         <v>16</v>
       </c>
-      <c r="F189">
+      <c r="F189" t="s">
+        <v>44</v>
+      </c>
+      <c r="G189">
         <v>165583</v>
       </c>
-      <c r="G189">
+      <c r="H189">
         <v>490000</v>
       </c>
-      <c r="H189">
+      <c r="I189">
         <v>1142982</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>33</v>
       </c>
@@ -4636,17 +5216,20 @@
       <c r="E190" t="s">
         <v>17</v>
       </c>
-      <c r="F190">
+      <c r="F190" t="s">
+        <v>44</v>
+      </c>
+      <c r="G190">
         <v>165583</v>
       </c>
-      <c r="G190">
+      <c r="H190">
         <v>399808</v>
       </c>
-      <c r="H190">
+      <c r="I190">
         <v>238647</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -4659,17 +5242,20 @@
       <c r="E191" t="s">
         <v>18</v>
       </c>
-      <c r="F191">
+      <c r="F191" t="s">
+        <v>44</v>
+      </c>
+      <c r="G191">
         <v>165583</v>
       </c>
-      <c r="G191">
+      <c r="H191">
         <v>399808</v>
       </c>
-      <c r="H191">
+      <c r="I191">
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>33</v>
       </c>
@@ -4682,17 +5268,20 @@
       <c r="E192" t="s">
         <v>19</v>
       </c>
-      <c r="F192">
+      <c r="F192" t="s">
+        <v>44</v>
+      </c>
+      <c r="G192">
         <v>165583</v>
       </c>
-      <c r="G192">
+      <c r="H192">
         <v>449808</v>
       </c>
-      <c r="H192">
+      <c r="I192">
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -4705,17 +5294,21 @@
       <c r="E193" t="s">
         <v>20</v>
       </c>
-      <c r="F193">
+      <c r="F193" t="s">
+        <v>44</v>
+      </c>
+      <c r="G193">
         <v>165583</v>
       </c>
-      <c r="G193">
+      <c r="H193">
         <v>399808</v>
       </c>
-      <c r="H193">
+      <c r="I193">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4724,8 +5317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>